<commit_message>
updated data file so that anything measured by area now gives a density of number of cm2 covered per m2. also added a figure showing mean density of taxa across the different stages
</commit_message>
<xml_diff>
--- a/data/taxon_count_data_internal_pipework.xlsx
+++ b/data/taxon_count_data_internal_pipework.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arlie/Documents/PhD_work/Chapters_thesis_papers/5 Internal_Pipework/internal_pipework/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E53E8D9-CD1F-3348-9CA6-AA3F56CAC727}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEE3435C-3DA5-F94A-9B0D-968A88D97508}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="21900" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5920" yWindow="1660" windowWidth="25040" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$R$759</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -2181,8 +2184,8 @@
   <dimension ref="A1:R759"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A733" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E720" sqref="E720:E731"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2900,7 +2903,7 @@
         <v>27</v>
       </c>
       <c r="E16" t="str">
-        <f t="shared" ref="E16:E79" si="1">_xlfn.CONCAT(M16, "_",N16)</f>
+        <f t="shared" ref="E16:E77" si="1">_xlfn.CONCAT(M16, "_",N16)</f>
         <v>loose_4</v>
       </c>
       <c r="F16">
@@ -6253,7 +6256,7 @@
         <v>73</v>
       </c>
       <c r="E82" t="str">
-        <f t="shared" ref="E80:E143" si="3">_xlfn.CONCAT(M82, "_",N82)</f>
+        <f t="shared" ref="E82:E143" si="3">_xlfn.CONCAT(M82, "_",N82)</f>
         <v>loose_1</v>
       </c>
       <c r="F82">
@@ -25055,7 +25058,7 @@
         <v>424</v>
       </c>
       <c r="E464" t="str">
-        <f t="shared" ref="E464:E527" si="15">_xlfn.CONCAT(M464, "_",N464)</f>
+        <f t="shared" ref="E464:E504" si="15">_xlfn.CONCAT(M464, "_",N464)</f>
         <v>bryozoan_5</v>
       </c>
       <c r="F464">
@@ -28761,7 +28764,7 @@
         <v>209</v>
       </c>
       <c r="E547" t="str">
-        <f t="shared" ref="E528:E591" si="17">_xlfn.CONCAT(M547, "_",N547)</f>
+        <f t="shared" ref="E547:E591" si="17">_xlfn.CONCAT(M547, "_",N547)</f>
         <v>loose_1</v>
       </c>
       <c r="F547">
@@ -35361,7 +35364,7 @@
         <v>16</v>
       </c>
       <c r="G676">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H676">
         <v>1</v>
@@ -35658,7 +35661,7 @@
         <v>8</v>
       </c>
       <c r="G683">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H683">
         <v>1</v>
@@ -35913,7 +35916,7 @@
         <v>12</v>
       </c>
       <c r="G689">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H689">
         <v>1</v>
@@ -36010,7 +36013,7 @@
         <v>2</v>
       </c>
       <c r="G691">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H691">
         <v>1</v>
@@ -37535,7 +37538,7 @@
         <v>14</v>
       </c>
       <c r="G720">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H720">
         <v>1</v>
@@ -38048,7 +38051,7 @@
         <v>180</v>
       </c>
       <c r="E732" t="str">
-        <f t="shared" ref="E720:E759" si="23">_xlfn.CONCAT(M732, "_",N732)</f>
+        <f t="shared" ref="E732:E759" si="23">_xlfn.CONCAT(M732, "_",N732)</f>
         <v>loose_1</v>
       </c>
       <c r="F732">

</xml_diff>